<commit_message>
Pass orthogonalization parameters to OrthogonalizationInitialize
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15263082-01F7-4EF9-8647-6BFC533E3BF9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D3ECE2-386D-45CF-B33A-70BC7BE2D565}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed MakePath in LandBoundaries
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751EFB6C-3206-4FE3-BCAF-2646357025D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F5B021-2C23-4F17-8862-77C62D431A89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>D</t>
   </si>
@@ -196,13 +196,23 @@
   <si>
     <t>Team member (code reviews)</t>
   </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -355,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -374,6 +384,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1038,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
@@ -1063,6 +1074,37 @@
         <v>1800</v>
       </c>
       <c r="H18" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <f>24480/135</f>
+        <v>181.33333333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <f>8+34</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <f>B21-B22</f>
+        <v>139.33333333333334</v>
+      </c>
+      <c r="C23" s="16">
+        <f>(B21-B22)/B21*100</f>
+        <v>76.838235294117652</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1074,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bug fix in landboundaries correct OneCrossingLandBoundary test
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F5B021-2C23-4F17-8862-77C62D431A89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56906EBB-2CEA-4BB3-9EEB-E7557E478086}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,8 +1089,8 @@
         <v>52</v>
       </c>
       <c r="B22">
-        <f>8+34</f>
-        <v>42</v>
+        <f>8+34+34+16</f>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1099,11 +1099,11 @@
       </c>
       <c r="B23">
         <f>B21-B22</f>
-        <v>139.33333333333334</v>
+        <v>89.333333333333343</v>
       </c>
       <c r="C23" s="16">
         <f>(B21-B22)/B21*100</f>
-        <v>76.838235294117652</v>
+        <v>49.264705882352942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First implementation of Splines
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7556F2-8A74-480A-9E63-189057900DD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3602D4-9457-406A-832B-5869D90A9578}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="1785" windowWidth="20730" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
     <sheet name="api calls" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -214,7 +214,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,13 +245,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -362,10 +374,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -385,8 +398,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,7 +745,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,52 +826,52 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="18">
         <f>F7+G7</f>
         <v>26</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="19">
         <f t="shared" ref="E7:E15" si="0">SUMPRODUCT(F$4:H$4,F7:H7)</f>
         <v>3440</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="18">
         <v>24</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="18">
         <f t="shared" ref="D8:D15" si="1">F8+G8</f>
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="19">
         <f t="shared" si="0"/>
         <v>1280</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="18">
         <v>8</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="18">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add SortedIndexes, ReorderVector renames GetSplineIntersections, GetSplineLength add spline properties
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3602D4-9457-406A-832B-5869D90A9578}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F1CB7-ED95-4B1E-9C5F-72474F2EFAA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +252,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +270,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -374,11 +386,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -403,9 +416,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -745,7 +764,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,27 +895,27 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="18">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="19">
         <f t="shared" si="0"/>
         <v>1280</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="18">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="18">
         <v>2</v>
       </c>
     </row>
@@ -926,27 +945,27 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="21">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="22">
         <f t="shared" si="0"/>
         <v>3440</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="21">
         <v>24</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="21">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add unit tests ComputeSplinesProperties, ComputeBoundingBox and test calculated intersections and m_maximumGridHeight
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++_phase2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F1CB7-ED95-4B1E-9C5F-72474F2EFAA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD21F50-4BCA-4194-9FC5-55A4A83F23B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="24270" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="begroting" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>D</t>
   </si>
@@ -391,7 +391,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -421,6 +421,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -764,7 +767,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,32 +923,32 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="21">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="22">
         <f t="shared" si="0"/>
         <v>4520</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="21">
         <v>32</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="23" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -958,7 +961,7 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <f t="shared" si="0"/>
         <v>3440</v>
       </c>

</xml_diff>